<commit_message>
Update first approach to excel variables
</commit_message>
<xml_diff>
--- a/resources/testing.xlsx
+++ b/resources/testing.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t xml:space="preserve">TestName</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Run</t>
   </si>
   <si>
-    <t xml:space="preserve">Var1</t>
+    <t xml:space="preserve">Account</t>
   </si>
   <si>
     <t xml:space="preserve">Var2</t>
@@ -37,28 +37,40 @@
     <t xml:space="preserve">Var3</t>
   </si>
   <si>
+    <t xml:space="preserve">AccountKO</t>
+  </si>
+  <si>
     <t xml:space="preserve">sample_apitests</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_mobiletests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_uitests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_apitests_excel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_mobiletests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_uitests</t>
+    <t xml:space="preserve">anxoportela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l324dsg34hguisito</t>
   </si>
 </sst>
 </file>
@@ -73,7 +85,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -96,6 +108,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,28 +160,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -183,79 +206,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="17.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="3" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="7.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working excel data retrieve and use in testcases
</commit_message>
<xml_diff>
--- a/resources/testing.xlsx
+++ b/resources/testing.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Api" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -85,7 +85,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -109,22 +109,41 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -132,6 +151,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -160,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,6 +212,34 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,16 +263,19 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="3" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="18.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="12.57"/>
@@ -232,76 +289,85 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="13" t="s">
         <v>10</v>
       </c>
+      <c r="F2" s="13"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="13" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update added all examples, edit documentation
</commit_message>
<xml_diff>
--- a/resources/testing.xlsx
+++ b/resources/testing.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t xml:space="preserve">TestName</t>
   </si>
@@ -39,16 +39,55 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">sample_apitests_excel</t>
+    <t xml:space="preserve">sample_apitests_exceldata</t>
   </si>
   <si>
     <t xml:space="preserve">anxoportela</t>
   </si>
   <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text_AssertionOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text_AssertionFail</t>
+  </si>
+  <si>
     <t xml:space="preserve">sample_mobiletests</t>
   </si>
   <si>
+    <t xml:space="preserve">Hola Mundo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adios Mundo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SearchFail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AssertionOK</t>
+  </si>
+  <si>
     <t xml:space="preserve">sample_uitests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_uitests_exceldata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repositories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">awesome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid repos</t>
   </si>
 </sst>
 </file>
@@ -164,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -206,6 +245,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,12 +274,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.55"/>
@@ -302,12 +345,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -315,8 +358,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="16.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.55"/>
@@ -337,17 +380,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -365,31 +433,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="7.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="14" style="1" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="7.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="13" style="1" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1021" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,17 +468,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Tree cleanup, improved settings and imports
</commit_message>
<xml_diff>
--- a/resources/testing.xlsx
+++ b/resources/testing.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t xml:space="preserve">TestName</t>
   </si>
@@ -30,19 +30,64 @@
     <t xml:space="preserve">Run</t>
   </si>
   <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_apitests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_apitests_exceldata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://api.github.com</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/anxoportela</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">token.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ourense, Spain</t>
+  </si>
+  <si>
     <t xml:space="preserve">Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_apitests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample_apitests_exceldata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anxoportela</t>
   </si>
   <si>
     <t xml:space="preserve">sample_mobiletests</t>
@@ -57,13 +102,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="168" formatCode="0"/>
-    <numFmt numFmtId="169" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="@"/>
+    <numFmt numFmtId="169" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -99,6 +144,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -158,46 +209,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,7 +284,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -226,67 +305,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="7.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="14" style="1" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="14.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="7.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="17" style="1" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://api.github.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -312,42 +420,42 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="7.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="14" style="1" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="10" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="12" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="10" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="13" width="7.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="14" style="10" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
+      <c r="C1" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="10"/>
+      <c r="A2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -375,42 +483,42 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="7.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="14" style="1" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="10" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="10" width="18.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="12" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="10" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="13" width="7.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="14" style="10" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
+      <c r="C1" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="10"/>
+      <c r="A2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>